<commit_message>
Primeira versão das movimentações aleatória e direcionada
</commit_message>
<xml_diff>
--- a/population2.xlsx
+++ b/population2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,13 +455,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.384967226523948</v>
+        <v>2.600125879871367</v>
       </c>
       <c r="C2" t="n">
-        <v>-48.66048129935654</v>
+        <v>-48.71384122723328</v>
       </c>
       <c r="D2" t="n">
-        <v>-17.74271500824575</v>
+        <v>-17.51148865412093</v>
       </c>
     </row>
     <row r="3">
@@ -469,13 +469,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2.463621964806639</v>
+        <v>2.128184125780414</v>
       </c>
       <c r="C3" t="n">
-        <v>-48.71384122723328</v>
+        <v>-48.6960545846077</v>
       </c>
       <c r="D3" t="n">
-        <v>-17.77828829349572</v>
+        <v>-17.76050165087074</v>
       </c>
     </row>
     <row r="4">
@@ -483,13 +483,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3.525638390344195</v>
+        <v>0.8842618317366855</v>
       </c>
       <c r="C4" t="n">
         <v>-48.68716126329491</v>
       </c>
       <c r="D4" t="n">
-        <v>-17.57374190330838</v>
+        <v>-17.75160832955824</v>
       </c>
     </row>
     <row r="5">
@@ -497,13 +497,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3.524741376763743</v>
+        <v>2.112953020975302</v>
       </c>
       <c r="C5" t="n">
-        <v>-48.70494790592049</v>
+        <v>-48.65158797804375</v>
       </c>
       <c r="D5" t="n">
-        <v>-17.74271500824575</v>
+        <v>-17.44034208362099</v>
       </c>
     </row>
     <row r="6">
@@ -511,13 +511,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2.964866165712742</v>
+        <v>1.999954430009206</v>
       </c>
       <c r="C6" t="n">
-        <v>-48.72273454854607</v>
+        <v>-48.67826794198212</v>
       </c>
       <c r="D6" t="n">
-        <v>-17.78718161480822</v>
+        <v>-17.57374190330838</v>
       </c>
     </row>
     <row r="7">
@@ -525,13 +525,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.228670862635628</v>
+        <v>1.227290394705522</v>
       </c>
       <c r="C7" t="n">
-        <v>-48.44704158784958</v>
+        <v>-48.67826794198212</v>
       </c>
       <c r="D7" t="n">
-        <v>-17.76939497218323</v>
+        <v>-17.6804617590583</v>
       </c>
     </row>
     <row r="8">
@@ -539,13 +539,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2.638501272196268</v>
+        <v>4.336656630291031</v>
       </c>
       <c r="C8" t="n">
-        <v>-48.67826794198212</v>
+        <v>-48.68716126329491</v>
       </c>
       <c r="D8" t="n">
-        <v>-17.73382168693326</v>
+        <v>-17.75160832955824</v>
       </c>
     </row>
     <row r="9">
@@ -553,13 +553,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.440458893559999</v>
+        <v>2.429556842686575</v>
       </c>
       <c r="C9" t="n">
-        <v>-48.67826794198212</v>
+        <v>-48.64269465673096</v>
       </c>
       <c r="D9" t="n">
-        <v>-17.76939497218323</v>
+        <v>-17.75160832955824</v>
       </c>
     </row>
     <row r="10">
@@ -567,13 +567,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02265169709643722</v>
+        <v>1.904204420047018</v>
       </c>
       <c r="C10" t="n">
-        <v>-48.6960545846077</v>
+        <v>-48.65158797804375</v>
       </c>
       <c r="D10" t="n">
-        <v>-17.79607493612071</v>
+        <v>-17.75160832955824</v>
       </c>
     </row>
     <row r="11">
@@ -581,13 +581,223 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2.785874714953448</v>
+        <v>3.104010962916469</v>
       </c>
       <c r="C11" t="n">
+        <v>-48.66048129935654</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-17.78718161480822</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.14687466333332</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-48.67826794198212</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-17.75160832955824</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3.349726232261484</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-48.65158797804375</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-17.75160832955824</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.875132332161531</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-48.66937462066933</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-17.74271500824575</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5625408548920923</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-48.72273454854607</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-17.78718161480822</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.078663903585458</v>
+      </c>
+      <c r="C16" t="n">
         <v>-48.6960545846077</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D16" t="n">
+        <v>-17.57374190330838</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.065614962453758</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-48.71384122723328</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-17.76050165087074</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3.550036750560322</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-48.66937462066933</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-17.76050165087074</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.672601942801667</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-48.72273454854607</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-17.79607493612071</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.383388957533608</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-48.68716126329491</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-17.79607493612071</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.169717741959055</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-48.71384122723328</v>
+      </c>
+      <c r="D21" t="n">
         <v>-17.75160832955824</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2.038109824454579</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-48.67826794198212</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-17.77828829349572</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2.556291383413752</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-48.66048129935654</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-17.75160832955824</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3.631499646315595</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-48.68716126329491</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-17.78718161480822</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.875028941637016</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-48.70494790592049</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-17.76050165087074</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.982599194667287</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-48.73162786985886</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-17.78718161480822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indivíduos aleatórios e orientados prontos, individuos com mémoria pronto somente o treino
</commit_message>
<xml_diff>
--- a/population2.xlsx
+++ b/population2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,13 +455,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.600125879871367</v>
+        <v>3.288106020426484</v>
       </c>
       <c r="C2" t="n">
-        <v>-48.71384122723328</v>
+        <v>-48.7849877977356</v>
       </c>
       <c r="D2" t="n">
-        <v>-17.51148865412093</v>
+        <v>-17.58263522462088</v>
       </c>
     </row>
     <row r="3">
@@ -469,13 +469,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2.128184125780414</v>
+        <v>1.51298247418209</v>
       </c>
       <c r="C3" t="n">
-        <v>-48.6960545846077</v>
+        <v>-48.35810837472168</v>
       </c>
       <c r="D3" t="n">
-        <v>-17.76050165087074</v>
+        <v>-17.47591536887096</v>
       </c>
     </row>
     <row r="4">
@@ -483,13 +483,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8842618317366855</v>
+        <v>1.883777508328557</v>
       </c>
       <c r="C4" t="n">
-        <v>-48.68716126329491</v>
+        <v>-48.75830783379723</v>
       </c>
       <c r="D4" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.92058143449561</v>
       </c>
     </row>
     <row r="5">
@@ -497,13 +497,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2.112953020975302</v>
+        <v>4.923052945892199</v>
       </c>
       <c r="C5" t="n">
-        <v>-48.65158797804375</v>
+        <v>-48.59822805016701</v>
       </c>
       <c r="D5" t="n">
-        <v>-17.44034208362099</v>
+        <v>-17.82275490005819</v>
       </c>
     </row>
     <row r="6">
@@ -511,13 +511,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.999954430009206</v>
+        <v>3.843117024035452</v>
       </c>
       <c r="C6" t="n">
-        <v>-48.67826794198212</v>
+        <v>-48.59822805016701</v>
       </c>
       <c r="D6" t="n">
-        <v>-17.57374190330838</v>
+        <v>-17.85832818530816</v>
       </c>
     </row>
     <row r="7">
@@ -525,13 +525,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.227290394705522</v>
+        <v>2.01599547980843</v>
       </c>
       <c r="C7" t="n">
-        <v>-48.67826794198212</v>
+        <v>-48.58933472885422</v>
       </c>
       <c r="D7" t="n">
-        <v>-17.6804617590583</v>
+        <v>-17.8049682574332</v>
       </c>
     </row>
     <row r="8">
@@ -539,13 +539,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>4.336656630291031</v>
+        <v>1.851458055775041</v>
       </c>
       <c r="C8" t="n">
-        <v>-48.68716126329491</v>
+        <v>-48.41146830259842</v>
       </c>
       <c r="D8" t="n">
-        <v>-17.75160832955824</v>
+        <v>-18.00951464762054</v>
       </c>
     </row>
     <row r="9">
@@ -553,13 +553,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.429556842686575</v>
+        <v>1.646281306401148</v>
       </c>
       <c r="C9" t="n">
-        <v>-48.64269465673096</v>
+        <v>-48.89170765348908</v>
       </c>
       <c r="D9" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.72492836562077</v>
       </c>
     </row>
     <row r="10">
@@ -567,13 +567,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.904204420047018</v>
+        <v>3.161720119650301</v>
       </c>
       <c r="C10" t="n">
-        <v>-48.65158797804375</v>
+        <v>-48.86502768955071</v>
       </c>
       <c r="D10" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.52038197543342</v>
       </c>
     </row>
     <row r="11">
@@ -581,13 +581,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>3.104010962916469</v>
+        <v>3.082147710257818</v>
       </c>
       <c r="C11" t="n">
-        <v>-48.66048129935654</v>
+        <v>-48.55376144360306</v>
       </c>
       <c r="D11" t="n">
-        <v>-17.78718161480822</v>
+        <v>-17.95615471974559</v>
       </c>
     </row>
     <row r="12">
@@ -595,13 +595,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.14687466333332</v>
+        <v>2.004023696749826</v>
       </c>
       <c r="C12" t="n">
-        <v>-48.67826794198212</v>
+        <v>-48.70494790592049</v>
       </c>
       <c r="D12" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.71603504430827</v>
       </c>
     </row>
     <row r="13">
@@ -609,13 +609,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>3.349726232261484</v>
+        <v>2.605731147626962</v>
       </c>
       <c r="C13" t="n">
-        <v>-48.65158797804375</v>
+        <v>-48.7849877977356</v>
       </c>
       <c r="D13" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.72492836562077</v>
       </c>
     </row>
     <row r="14">
@@ -623,13 +623,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2.875132332161531</v>
+        <v>3.037149219136999</v>
       </c>
       <c r="C14" t="n">
-        <v>-48.66937462066933</v>
+        <v>-48.429254945224</v>
       </c>
       <c r="D14" t="n">
-        <v>-17.74271500824575</v>
+        <v>-17.84054154268318</v>
       </c>
     </row>
     <row r="15">
@@ -637,13 +637,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5625408548920923</v>
+        <v>1.82176068413053</v>
       </c>
       <c r="C15" t="n">
-        <v>-48.72273454854607</v>
+        <v>-48.429254945224</v>
       </c>
       <c r="D15" t="n">
-        <v>-17.78718161480822</v>
+        <v>-17.95615471974559</v>
       </c>
     </row>
     <row r="16">
@@ -651,13 +651,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.078663903585458</v>
+        <v>2.563767901486071</v>
       </c>
       <c r="C16" t="n">
-        <v>-48.6960545846077</v>
+        <v>-48.35810837472168</v>
       </c>
       <c r="D16" t="n">
-        <v>-17.57374190330838</v>
+        <v>-17.74271500824575</v>
       </c>
     </row>
     <row r="17">
@@ -665,13 +665,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2.065614962453758</v>
+        <v>3.728649466520357</v>
       </c>
       <c r="C17" t="n">
-        <v>-48.71384122723328</v>
+        <v>-48.82056108298676</v>
       </c>
       <c r="D17" t="n">
-        <v>-17.76050165087074</v>
+        <v>-17.94726139843309</v>
       </c>
     </row>
     <row r="18">
@@ -679,13 +679,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3.550036750560322</v>
+        <v>2.808596721422223</v>
       </c>
       <c r="C18" t="n">
-        <v>-48.66937462066933</v>
+        <v>-48.93617426005303</v>
       </c>
       <c r="D18" t="n">
-        <v>-17.76050165087074</v>
+        <v>-17.57374190330838</v>
       </c>
     </row>
     <row r="19">
@@ -693,13 +693,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.672601942801667</v>
+        <v>2.096578190699095</v>
       </c>
       <c r="C19" t="n">
-        <v>-48.72273454854607</v>
+        <v>-48.81166776167397</v>
       </c>
       <c r="D19" t="n">
-        <v>-17.79607493612071</v>
+        <v>-17.66267511643331</v>
       </c>
     </row>
     <row r="20">
@@ -707,13 +707,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>2.383388957533608</v>
+        <v>1.712510194207048</v>
       </c>
       <c r="C20" t="n">
-        <v>-48.68716126329491</v>
+        <v>-48.7849877977356</v>
       </c>
       <c r="D20" t="n">
-        <v>-17.79607493612071</v>
+        <v>-17.90279479187063</v>
       </c>
     </row>
     <row r="21">
@@ -721,13 +721,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2.169717741959055</v>
+        <v>3.316342381388262</v>
       </c>
       <c r="C21" t="n">
-        <v>-48.71384122723328</v>
+        <v>-48.9628542239914</v>
       </c>
       <c r="D21" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.84054154268318</v>
       </c>
     </row>
     <row r="22">
@@ -735,13 +735,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>2.038109824454579</v>
+        <v>4.492538213535018</v>
       </c>
       <c r="C22" t="n">
-        <v>-48.67826794198212</v>
+        <v>-48.74941451248444</v>
       </c>
       <c r="D22" t="n">
-        <v>-17.77828829349572</v>
+        <v>-17.85832818530816</v>
       </c>
     </row>
     <row r="23">
@@ -749,13 +749,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>2.556291383413752</v>
+        <v>3.402387609134351</v>
       </c>
       <c r="C23" t="n">
-        <v>-48.66048129935654</v>
+        <v>-48.94506758136582</v>
       </c>
       <c r="D23" t="n">
-        <v>-17.75160832955824</v>
+        <v>-17.44034208362099</v>
       </c>
     </row>
     <row r="24">
@@ -763,13 +763,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>3.631499646315595</v>
+        <v>2.591741004210808</v>
       </c>
       <c r="C24" t="n">
-        <v>-48.68716126329491</v>
+        <v>-48.41146830259842</v>
       </c>
       <c r="D24" t="n">
-        <v>-17.78718161480822</v>
+        <v>-18.05398125418301</v>
       </c>
     </row>
     <row r="25">
@@ -777,13 +777,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.875028941637016</v>
+        <v>2.326881746831508</v>
       </c>
       <c r="C25" t="n">
-        <v>-48.70494790592049</v>
+        <v>-48.6960545846077</v>
       </c>
       <c r="D25" t="n">
-        <v>-17.76050165087074</v>
+        <v>-18.11623450337046</v>
       </c>
     </row>
     <row r="26">
@@ -791,13 +791,1063 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.982599194667287</v>
+        <v>3.135309916852812</v>
       </c>
       <c r="C26" t="n">
-        <v>-48.73162786985886</v>
+        <v>-48.74941451248444</v>
       </c>
       <c r="D26" t="n">
+        <v>-17.63599515249583</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.9791087204766298</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-48.89170765348908</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-17.83164822137068</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.851936796583082</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-48.86502768955071</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-17.44034208362099</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.825456240266661</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-48.52708147966469</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-17.92947475580811</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2.452947119468898</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-48.93617426005303</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-17.77828829349572</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3.449240383781877</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-48.9628542239914</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-17.96504804105808</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2.358748717335924</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-48.52708147966469</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-17.92947475580811</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2.58209295690031</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-48.58933472885422</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-18.01840796893304</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3.461545694918466</v>
+      </c>
+      <c r="C34" t="n">
+        <v>-48.80277444036118</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-18.10734118205797</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.27274143919668</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-48.53597480097748</v>
+      </c>
+      <c r="D35" t="n">
+        <v>-17.91168811318312</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.638594512444688</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-48.8739210108635</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-17.8138615787457</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.032051482319427</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-48.90949429611466</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-17.72492836562077</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>3.465873388958907</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-49.0517874371193</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-17.92058143449561</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.303171923967536</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-48.62490801410538</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-17.86722150662066</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.207068268210054</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-48.82945440429955</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-17.64488847380833</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.892756981831935</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-48.41146830259842</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-17.72492836562077</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.550852498228722</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-48.71384122723328</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-17.47591536887096</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.133571687366682</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-48.75830783379723</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-17.95615471974559</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.509072822040202</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-48.35810837472168</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-17.85832818530816</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2.236721209423012</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-48.88281433217629</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-17.79607493612071</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1.821678698694174</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-49.03400079449372</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-17.5470619393709</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2.183406817243628</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-49.0517874371193</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-18.08955453943299</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>3.053089169705205</v>
+      </c>
+      <c r="C48" t="n">
+        <v>-48.49150819441353</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-17.87611482793315</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>2.68517929341674</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-49.03400079449372</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-17.97394136237057</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2.828025522915642</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-48.6960545846077</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-17.73382168693326</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2.417861184289252</v>
+      </c>
+      <c r="C51" t="n">
+        <v>-48.86502768955071</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-17.71603504430827</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3.135610585039037</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-48.84724104692513</v>
+      </c>
+      <c r="D52" t="n">
         <v>-17.78718161480822</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2.598171306537652</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-48.46482823047516</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-17.52038197543342</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2.94023761920409</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-48.9628542239914</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-17.66267511643331</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>2.831521458814521</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-48.45593490916237</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-17.46702204755847</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2.630698332366048</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-48.36700169603447</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-17.50259533280844</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.964272030079466</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-49.01621415186814</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-18.05398125418301</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3.144034676027212</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-48.83834772561234</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-17.70714172299578</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.838432985259744</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-48.57154808622864</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-18.0628745754955</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.780299694408843</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-48.82945440429955</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-18.11623450337046</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.374906316610484</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-48.40257498128563</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-17.73382168693326</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.2655497512457119</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-48.59822805016701</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-17.51148865412093</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.550583234896159</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-48.38478833866005</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-17.49370201149594</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.55682949804464</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-48.66937462066933</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-17.5470619393709</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2.37120940518835</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-48.53597480097748</v>
+      </c>
+      <c r="D65" t="n">
+        <v>-17.53816861805841</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>2.425175262444463</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-48.74052119117165</v>
+      </c>
+      <c r="D66" t="n">
+        <v>-17.52927529674592</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2.781003531899271</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-48.35810837472168</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-17.92947475580811</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2.557263635638366</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-48.77609447642281</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-17.98283468368307</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>3.913888462044563</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-48.88281433217629</v>
+      </c>
+      <c r="D69" t="n">
+        <v>-18.11623450337046</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.084533474452634</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-48.70494790592049</v>
+      </c>
+      <c r="D70" t="n">
+        <v>-17.52927529674592</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2.390327108199596</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-48.42036162391121</v>
+      </c>
+      <c r="D71" t="n">
+        <v>-18.00951464762054</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.905816856521713</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-48.6960545846077</v>
+      </c>
+      <c r="D72" t="n">
+        <v>-17.98283468368307</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>3.760338873337174</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-48.50929483703911</v>
+      </c>
+      <c r="D73" t="n">
+        <v>-17.70714172299578</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>3.417059053542305</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-49.0517874371193</v>
+      </c>
+      <c r="D74" t="n">
+        <v>-18.0628745754955</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1.83345134658502</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-48.79388111904839</v>
+      </c>
+      <c r="D75" t="n">
+        <v>-17.60931518855836</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3.483352071168151</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-48.82945440429955</v>
+      </c>
+      <c r="D76" t="n">
+        <v>-18.03619461155802</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2.769976451271307</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-48.36700169603447</v>
+      </c>
+      <c r="D77" t="n">
+        <v>-18.00062132630805</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2.367297002078284</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-48.61601469279259</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-17.99172800499556</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2.499827292266382</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-48.9628542239914</v>
+      </c>
+      <c r="D79" t="n">
+        <v>-17.84943486399567</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3.011751188272821</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-48.44704158784958</v>
+      </c>
+      <c r="D80" t="n">
+        <v>-17.87611482793315</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2.518657372189519</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-48.62490801410538</v>
+      </c>
+      <c r="D81" t="n">
+        <v>-17.422555440996</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>3.181043825417906</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-48.5181881583519</v>
+      </c>
+      <c r="D82" t="n">
+        <v>-17.44923540493348</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>3.323384688600298</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-48.83834772561234</v>
+      </c>
+      <c r="D83" t="n">
+        <v>-17.9383680771206</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1.56261378354083</v>
+      </c>
+      <c r="C84" t="n">
+        <v>-48.36700169603447</v>
+      </c>
+      <c r="D84" t="n">
+        <v>-17.64488847380833</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>2.156503423199001</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-48.82945440429955</v>
+      </c>
+      <c r="D85" t="n">
+        <v>-17.88500814924564</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2.977658796332284</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-48.46482823047516</v>
+      </c>
+      <c r="D86" t="n">
+        <v>-17.51148865412093</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>1.091111278706914</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-48.429254945224</v>
+      </c>
+      <c r="D87" t="n">
+        <v>-17.90279479187063</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>3.535223860752818</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-48.91838761742745</v>
+      </c>
+      <c r="D88" t="n">
+        <v>-17.52038197543342</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>1.438574765742887</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-49.02510747318093</v>
+      </c>
+      <c r="D89" t="n">
+        <v>-17.95615471974559</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>3.748650233318034</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-48.85613436823792</v>
+      </c>
+      <c r="D90" t="n">
+        <v>-18.10734118205797</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2.88811527821489</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-48.74052119117165</v>
+      </c>
+      <c r="D91" t="n">
+        <v>-17.84943486399567</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2.51419465954986</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-48.80277444036118</v>
+      </c>
+      <c r="D92" t="n">
+        <v>-18.03619461155802</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>3.24576132082941</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-48.99842750924256</v>
+      </c>
+      <c r="D93" t="n">
+        <v>-17.45812872624597</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2.227594892819464</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-48.71384122723328</v>
+      </c>
+      <c r="D94" t="n">
+        <v>-17.84054154268318</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>1.629063704173762</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-48.82056108298676</v>
+      </c>
+      <c r="D95" t="n">
+        <v>-17.76939497218323</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1.835069738207439</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-48.89170765348908</v>
+      </c>
+      <c r="D96" t="n">
+        <v>-18.09844786074548</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>2.799914223925677</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-48.9628542239914</v>
+      </c>
+      <c r="D97" t="n">
+        <v>-17.74271500824575</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2.633971983761162</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-48.61601469279259</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-17.66267511643331</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2.213985648905231</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-48.54486812229027</v>
+      </c>
+      <c r="D99" t="n">
+        <v>-18.05398125418301</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2.29968972396831</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-48.68716126329491</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-17.74271500824575</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>2.743266950628115</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-48.45593490916237</v>
+      </c>
+      <c r="D101" t="n">
+        <v>-17.68935508037079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do modelo de movimentação baseado em memória e do gerador de paisagens que agora crias os rasters na resolução desejada
</commit_message>
<xml_diff>
--- a/population2.xlsx
+++ b/population2.xlsx
@@ -455,13 +455,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.857456349141684</v>
+        <v>3.639357264516869</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1272727272727273</v>
+        <v>0.8909090909090909</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2181818181818183</v>
+        <v>0.8181818181818181</v>
       </c>
     </row>
     <row r="3">
@@ -469,13 +469,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2.82316008435684</v>
+        <v>1.267300926324749</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2818181818181819</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4">
@@ -483,13 +483,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2.034556225376642</v>
+        <v>1.036731823133914</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5818181818181818</v>
+        <v>0.2909090909090909</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6909090909090909</v>
+        <v>0.7181818181818183</v>
       </c>
     </row>
     <row r="5">
@@ -497,13 +497,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2.312938648328651</v>
+        <v>2.346932117483861</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6454545454545454</v>
+        <v>0.5</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.1363636363636364</v>
       </c>
     </row>
     <row r="6">
@@ -511,13 +511,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3.257410029238286</v>
+        <v>2.994319709317411</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6545454545454545</v>
+        <v>0.2363636363636364</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9636363636363636</v>
+        <v>0.8272727272727273</v>
       </c>
     </row>
     <row r="7">
@@ -525,13 +525,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.911803268236926</v>
+        <v>2.628161784490352</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2272727272727273</v>
+        <v>0.3727272727272727</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.2818181818181819</v>
       </c>
     </row>
     <row r="8">
@@ -539,13 +539,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>3.943104066947778</v>
+        <v>1.956867103089487</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3272727272727273</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="D8" t="n">
-        <v>0.06363636363636371</v>
+        <v>0.3090909090909091</v>
       </c>
     </row>
     <row r="9">
@@ -553,13 +553,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.526618811935275</v>
+        <v>2.221315499852857</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8818181818181817</v>
+        <v>0.5727272727272728</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5545454545454546</v>
+        <v>0.2454545454545455</v>
       </c>
     </row>
     <row r="10">
@@ -567,13 +567,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2.882709767312208</v>
+        <v>3.210639168481903</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9636363636363636</v>
+        <v>0.6272727272727272</v>
       </c>
       <c r="D10" t="n">
-        <v>0.06363636363636371</v>
+        <v>0.6818181818181819</v>
       </c>
     </row>
     <row r="11">
@@ -581,13 +581,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2.94173190460436</v>
+        <v>0.5490662632377095</v>
       </c>
       <c r="C11" t="n">
-        <v>0.00909090909090909</v>
+        <v>0.9181818181818181</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5272727272727273</v>
+        <v>0.9454545454545454</v>
       </c>
     </row>
     <row r="12">
@@ -595,13 +595,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2.657193824460562</v>
+        <v>1.536370198059503</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3545454545454546</v>
+        <v>0.2181818181818182</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.3727272727272728</v>
       </c>
     </row>
     <row r="13">
@@ -609,13 +609,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>4.180317650523203</v>
+        <v>1.396572294386483</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6272727272727272</v>
+        <v>0.2454545454545455</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5</v>
+        <v>0.03636363636363638</v>
       </c>
     </row>
     <row r="14">
@@ -623,13 +623,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>3.421713048934853</v>
+        <v>3.316944508690913</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2909090909090909</v>
+        <v>0.03636363636363638</v>
       </c>
     </row>
     <row r="15">
@@ -637,13 +637,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>3.425333240032497</v>
+        <v>3.721807109487508</v>
       </c>
       <c r="C15" t="n">
-        <v>0.08181818181818182</v>
+        <v>0.5363636363636364</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9636363636363636</v>
+        <v>0.1909090909090909</v>
       </c>
     </row>
     <row r="16">
@@ -651,13 +651,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.052199023448932</v>
+        <v>1.990433615503845</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8363636363636363</v>
+        <v>0.5363636363636364</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3363636363636364</v>
+        <v>0.7727272727272727</v>
       </c>
     </row>
     <row r="17">
@@ -665,13 +665,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>3.802466715640479</v>
+        <v>0.7216216206363824</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9181818181818181</v>
+        <v>0.4181818181818182</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8090909090909091</v>
+        <v>0.1363636363636364</v>
       </c>
     </row>
     <row r="18">
@@ -679,13 +679,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2.885793231064412</v>
+        <v>1.649746323567624</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9454545454545454</v>
+        <v>0.1272727272727273</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2636363636363637</v>
+        <v>0.3363636363636364</v>
       </c>
     </row>
     <row r="19">
@@ -693,13 +693,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2.269103974089747</v>
+        <v>2.211936483046026</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3818181818181818</v>
+        <v>0.3454545454545455</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2090909090909091</v>
+        <v>0.1090909090909091</v>
       </c>
     </row>
     <row r="20">
@@ -707,13 +707,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.248187657800693</v>
+        <v>3.558903765998242</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3818181818181818</v>
+        <v>0.4636363636363636</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2181818181818183</v>
+        <v>0.3363636363636364</v>
       </c>
     </row>
     <row r="21">
@@ -721,13 +721,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2.286875979213454</v>
+        <v>2.052472253384159</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4636363636363636</v>
+        <v>0.9272727272727272</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6090909090909091</v>
+        <v>0.5818181818181818</v>
       </c>
     </row>
     <row r="22">
@@ -735,13 +735,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>4.43528367073663</v>
+        <v>1.908738155791507</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2</v>
+        <v>0.8272727272727273</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7</v>
+        <v>0.6818181818181819</v>
       </c>
     </row>
     <row r="23">
@@ -749,13 +749,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.602268719275745</v>
+        <v>1.752570065567825</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4727272727272727</v>
+        <v>0.5545454545454546</v>
       </c>
       <c r="D23" t="n">
-        <v>0.009090909090909149</v>
+        <v>0.4363636363636364</v>
       </c>
     </row>
     <row r="24">
@@ -763,13 +763,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>2.684756887966497</v>
+        <v>1.356084410781417</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7181818181818181</v>
+        <v>0.08181818181818182</v>
       </c>
       <c r="D24" t="n">
-        <v>0.1727272727272727</v>
+        <v>0.04545454545454553</v>
       </c>
     </row>
     <row r="25">
@@ -777,13 +777,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>2.274491265508628</v>
+        <v>1.904446878351196</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6181818181818182</v>
+        <v>0.6454545454545454</v>
       </c>
       <c r="D25" t="n">
-        <v>0.1000000000000001</v>
+        <v>0.3090909090909091</v>
       </c>
     </row>
     <row r="26">
@@ -791,13 +791,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>2.821590166724934</v>
+        <v>1.985971858623564</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5818181818181818</v>
+        <v>0.7545454545454545</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3090909090909091</v>
+        <v>0.7545454545454545</v>
       </c>
     </row>
     <row r="27">
@@ -805,13 +805,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>2.447600590809197</v>
+        <v>2.616714026348632</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.5818181818181818</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4636363636363636</v>
+        <v>0.1818181818181819</v>
       </c>
     </row>
     <row r="28">
@@ -819,13 +819,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.349310376743624</v>
+        <v>2.894649102499058</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.9363636363636363</v>
       </c>
       <c r="D28" t="n">
-        <v>0.9727272727272728</v>
+        <v>0.5272727272727273</v>
       </c>
     </row>
     <row r="29">
@@ -833,13 +833,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.617618788327995</v>
+        <v>2.16766252887999</v>
       </c>
       <c r="C29" t="n">
-        <v>0.5363636363636364</v>
+        <v>0.6727272727272727</v>
       </c>
       <c r="D29" t="n">
-        <v>0.1181818181818183</v>
+        <v>0.7090909090909091</v>
       </c>
     </row>
     <row r="30">
@@ -847,13 +847,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.862255769537647</v>
+        <v>3.153741985409201</v>
       </c>
       <c r="C30" t="n">
         <v>0.3090909090909091</v>
       </c>
       <c r="D30" t="n">
-        <v>0.6909090909090909</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="31">
@@ -861,13 +861,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>2.777579931477052</v>
+        <v>1.928829294193834</v>
       </c>
       <c r="C31" t="n">
-        <v>0.8272727272727273</v>
+        <v>0.4909090909090909</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3</v>
+        <v>0.2454545454545455</v>
       </c>
     </row>
     <row r="32">
@@ -875,13 +875,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.519973443222006</v>
+        <v>1.63125418964535</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7181818181818181</v>
+        <v>0.3545454545454546</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8363636363636364</v>
+        <v>0.8636363636363636</v>
       </c>
     </row>
     <row r="33">
@@ -889,13 +889,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>2.387276315380739</v>
+        <v>1.972969181088311</v>
       </c>
       <c r="C33" t="n">
-        <v>0.7</v>
+        <v>0.5909090909090908</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2636363636363637</v>
+        <v>0.04545454545454553</v>
       </c>
     </row>
     <row r="34">
@@ -903,13 +903,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>2.631286436953711</v>
+        <v>2.2614534407422</v>
       </c>
       <c r="C34" t="n">
-        <v>0.4090909090909091</v>
+        <v>0.8545454545454545</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9727272727272728</v>
+        <v>0.3181818181818182</v>
       </c>
     </row>
     <row r="35">
@@ -917,13 +917,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>2.668677933260819</v>
+        <v>3.020645444184856</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1363636363636364</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="D35" t="n">
-        <v>0.7818181818181819</v>
+        <v>0.06363636363636371</v>
       </c>
     </row>
     <row r="36">
@@ -931,13 +931,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>3.360551971664565</v>
+        <v>1.430288620498196</v>
       </c>
       <c r="C36" t="n">
-        <v>0.3090909090909091</v>
+        <v>0.2545454545454545</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1727272727272727</v>
+        <v>0.7272727272727273</v>
       </c>
     </row>
     <row r="37">
@@ -945,13 +945,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>2.831249492923973</v>
+        <v>1.73049082626007</v>
       </c>
       <c r="C37" t="n">
-        <v>0.03636363636363636</v>
+        <v>0.609090909090909</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5</v>
+        <v>0.7181818181818183</v>
       </c>
     </row>
     <row r="38">
@@ -959,13 +959,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>2.540814120480723</v>
+        <v>3.097541125975837</v>
       </c>
       <c r="C38" t="n">
-        <v>0.5</v>
+        <v>0.9545454545454545</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3</v>
+        <v>0.2181818181818183</v>
       </c>
     </row>
     <row r="39">
@@ -973,13 +973,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.804267288583436</v>
+        <v>2.664868520100121</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1545454545454545</v>
+        <v>0.609090909090909</v>
       </c>
       <c r="D39" t="n">
-        <v>0.1545454545454545</v>
+        <v>0.1090909090909091</v>
       </c>
     </row>
     <row r="40">
@@ -987,13 +987,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>3.778981359621451</v>
+        <v>2.872891472105213</v>
       </c>
       <c r="C40" t="n">
-        <v>0.02727272727272727</v>
+        <v>0.3090909090909091</v>
       </c>
       <c r="D40" t="n">
-        <v>0.9</v>
+        <v>0.490909090909091</v>
       </c>
     </row>
     <row r="41">
@@ -1001,13 +1001,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>2.810843311463718</v>
+        <v>2.847233275282147</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1636363636363636</v>
+        <v>0.4818181818181818</v>
       </c>
       <c r="D41" t="n">
-        <v>0.1909090909090909</v>
+        <v>0.7090909090909091</v>
       </c>
     </row>
     <row r="42">
@@ -1015,13 +1015,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>2.430184294799532</v>
+        <v>1.884788789239989</v>
       </c>
       <c r="C42" t="n">
-        <v>0.509090909090909</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3545454545454546</v>
+        <v>0.7090909090909091</v>
       </c>
     </row>
     <row r="43">
@@ -1029,13 +1029,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.407199962447356</v>
+        <v>2.052136444473186</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6909090909090909</v>
+        <v>0.9454545454545454</v>
       </c>
       <c r="D43" t="n">
-        <v>0.4636363636363636</v>
+        <v>0.1000000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -1043,13 +1043,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>2.459543328747059</v>
+        <v>1.670744220891262</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9909090909090909</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="D44" t="n">
-        <v>0.6272727272727273</v>
+        <v>0.7181818181818183</v>
       </c>
     </row>
     <row r="45">
@@ -1057,13 +1057,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.918411796969492</v>
+        <v>0.7968207385319868</v>
       </c>
       <c r="C45" t="n">
-        <v>0.7090909090909091</v>
+        <v>0.5181818181818182</v>
       </c>
       <c r="D45" t="n">
-        <v>0.4727272727272728</v>
+        <v>0.7181818181818183</v>
       </c>
     </row>
     <row r="46">
@@ -1071,13 +1071,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>2.665126108045687</v>
+        <v>2.414704811449499</v>
       </c>
       <c r="C46" t="n">
-        <v>0.7181818181818181</v>
+        <v>0.4363636363636363</v>
       </c>
       <c r="D46" t="n">
-        <v>0.1454545454545455</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="47">
@@ -1085,13 +1085,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>3.388544194951257</v>
+        <v>3.637041109218055</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9181818181818181</v>
+        <v>0.5727272727272728</v>
       </c>
       <c r="D47" t="n">
-        <v>0.8727272727272728</v>
+        <v>0.2181818181818183</v>
       </c>
     </row>
     <row r="48">
@@ -1099,13 +1099,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>2.724534498756279</v>
+        <v>1.799200636417428</v>
       </c>
       <c r="C48" t="n">
-        <v>0.5363636363636364</v>
+        <v>0.7454545454545454</v>
       </c>
       <c r="D48" t="n">
-        <v>0.8181818181818181</v>
+        <v>0.04545454545454553</v>
       </c>
     </row>
     <row r="49">
@@ -1113,13 +1113,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.956697960103244</v>
+        <v>2.617465268312308</v>
       </c>
       <c r="C49" t="n">
-        <v>0.6727272727272727</v>
+        <v>0.1363636363636364</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2272727272727273</v>
+        <v>0.2727272727272727</v>
       </c>
     </row>
     <row r="50">
@@ -1127,13 +1127,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>3.015420137878876</v>
+        <v>2.549483547470375</v>
       </c>
       <c r="C50" t="n">
-        <v>0.8272727272727273</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="D50" t="n">
-        <v>0.1636363636363637</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="51">
@@ -1141,13 +1141,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.654166768088889</v>
+        <v>2.166045691038782</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8090909090909091</v>
+        <v>0.8545454545454545</v>
       </c>
       <c r="D51" t="n">
-        <v>0.1090909090909091</v>
+        <v>0.5636363636363637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>